<commit_message>
Added algorithm for assigning machines and workers to routes
</commit_message>
<xml_diff>
--- a/ProductionData.xlsx
+++ b/ProductionData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programy\MyProject\JobFlowScheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CC2349-88E2-4CD3-8B82-3A13AD3C379B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C5AFB7-C04F-42CC-831F-545B8B889E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="856" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="856" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PRACOWNICY" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="124">
   <si>
     <t>IMIE</t>
   </si>
@@ -295,24 +295,6 @@
     <t>SYMBOL_GNIAZDA</t>
   </si>
   <si>
-    <t>M5322</t>
-  </si>
-  <si>
-    <t>M8072</t>
-  </si>
-  <si>
-    <t>M8606</t>
-  </si>
-  <si>
-    <t>M5323</t>
-  </si>
-  <si>
-    <t>M8073</t>
-  </si>
-  <si>
-    <t>M8607</t>
-  </si>
-  <si>
     <t>ID_OPERACJI</t>
   </si>
   <si>
@@ -331,13 +313,103 @@
     <t>KF02KS10</t>
   </si>
   <si>
-    <t>M1607</t>
-  </si>
-  <si>
     <t>PHILIPS p230</t>
   </si>
   <si>
     <t>PHILIPS p250</t>
+  </si>
+  <si>
+    <t>P2014</t>
+  </si>
+  <si>
+    <t>P2015</t>
+  </si>
+  <si>
+    <t>P2016</t>
+  </si>
+  <si>
+    <t>P2017</t>
+  </si>
+  <si>
+    <t>P2018</t>
+  </si>
+  <si>
+    <t>P2019</t>
+  </si>
+  <si>
+    <t>P2020</t>
+  </si>
+  <si>
+    <t>P2021</t>
+  </si>
+  <si>
+    <t>P2022</t>
+  </si>
+  <si>
+    <t>P2023</t>
+  </si>
+  <si>
+    <t>P2024</t>
+  </si>
+  <si>
+    <t>M5001</t>
+  </si>
+  <si>
+    <t>M5002</t>
+  </si>
+  <si>
+    <t>M5003</t>
+  </si>
+  <si>
+    <t>M5004</t>
+  </si>
+  <si>
+    <t>M5005</t>
+  </si>
+  <si>
+    <t>M5006</t>
+  </si>
+  <si>
+    <t>M5007</t>
+  </si>
+  <si>
+    <t>M5008</t>
+  </si>
+  <si>
+    <t>M5009</t>
+  </si>
+  <si>
+    <t>M5010</t>
+  </si>
+  <si>
+    <t>M5011</t>
+  </si>
+  <si>
+    <t>M5012</t>
+  </si>
+  <si>
+    <t>M5013</t>
+  </si>
+  <si>
+    <t>M5014</t>
+  </si>
+  <si>
+    <t>M5015</t>
+  </si>
+  <si>
+    <t>M5016</t>
+  </si>
+  <si>
+    <t>M5017</t>
+  </si>
+  <si>
+    <t>M5018</t>
+  </si>
+  <si>
+    <t>M5019</t>
+  </si>
+  <si>
+    <t>M5020</t>
   </si>
 </sst>
 </file>
@@ -701,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B1AF800-7C7B-4DA1-B9EF-A1DE1866A583}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,7 +815,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -813,7 +885,7 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -827,7 +899,7 @@
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -883,6 +955,160 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
         <v>80</v>
       </c>
     </row>
@@ -895,7 +1121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D91FF2-5DA7-4A7E-9F3A-77FC9995DA3E}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -919,7 +1145,7 @@
         <v>23</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>84</v>
@@ -937,7 +1163,7 @@
         <v>46</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1689,7 +1915,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
         <v>58</v>
@@ -1836,7 +2062,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
         <v>50</v>
@@ -1871,10 +2097,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A737D97F-C3F3-4EBB-935E-89B1E56B6C13}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1898,7 +2124,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
         <v>63</v>
@@ -1909,7 +2135,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
@@ -1920,7 +2146,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
         <v>62</v>
@@ -1931,7 +2157,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
@@ -1942,7 +2168,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
         <v>63</v>
@@ -1953,7 +2179,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
         <v>62</v>
@@ -1964,7 +2190,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
         <v>63</v>
@@ -1975,7 +2201,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="B9" t="s">
         <v>63</v>
@@ -1986,7 +2212,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="B10" t="s">
         <v>62</v>
@@ -1997,24 +2223,145 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="B11" t="s">
         <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="B12" t="s">
         <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>99</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2024,10 +2371,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63ECF564-DD6A-47B3-9FA7-B9A0B7520F7A}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A7" sqref="A7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2063,35 +2410,35 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B3" s="4">
-        <v>43225</v>
+        <v>43198</v>
       </c>
       <c r="C3" s="4">
-        <v>43256</v>
+        <v>43228</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" s="4">
-        <v>43137</v>
+        <v>43109</v>
       </c>
       <c r="C4" s="4">
-        <v>43165</v>
+        <v>43140</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" s="4">
-        <v>43198</v>
+        <v>43170</v>
       </c>
       <c r="C5" s="4">
-        <v>43228</v>
+        <v>43201</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -2099,54 +2446,10 @@
         <v>54</v>
       </c>
       <c r="B6" s="4">
-        <v>43109</v>
+        <v>43112</v>
       </c>
       <c r="C6" s="4">
-        <v>43140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="4">
-        <v>43261</v>
-      </c>
-      <c r="C7" s="4">
-        <v>43291</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="4">
-        <v>43170</v>
-      </c>
-      <c r="C8" s="4">
-        <v>43201</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="4">
-        <v>43112</v>
-      </c>
-      <c r="C9" s="4">
         <v>43143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="4">
-        <v>43193</v>
-      </c>
-      <c r="C10" s="4">
-        <v>43223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wydzielenie kodu do osobnych klas
</commit_message>
<xml_diff>
--- a/ProductionData.xlsx
+++ b/ProductionData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programy\MyProject\JobFlowScheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C5AFB7-C04F-42CC-831F-545B8B889E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0985153F-0ABC-4203-A991-F0DA36B6735A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="856" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="856" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PRACOWNICY" sheetId="2" r:id="rId1"/>
@@ -1947,7 +1947,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1976,10 +1976,10 @@
         <v>67</v>
       </c>
       <c r="B2" s="4">
-        <v>43198</v>
+        <v>45499</v>
       </c>
       <c r="C2" s="4">
-        <v>43228</v>
+        <v>45504</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1987,10 +1987,10 @@
         <v>71</v>
       </c>
       <c r="B3" s="4">
-        <v>43109</v>
+        <v>45441</v>
       </c>
       <c r="C3" s="4">
-        <v>43140</v>
+        <v>45443</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1998,10 +1998,10 @@
         <v>72</v>
       </c>
       <c r="B4" s="4">
-        <v>43261</v>
+        <v>45536</v>
       </c>
       <c r="C4" s="4">
-        <v>43291</v>
+        <v>45539</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2009,10 +2009,10 @@
         <v>73</v>
       </c>
       <c r="B5" s="4">
-        <v>43170</v>
+        <v>45542</v>
       </c>
       <c r="C5" s="4">
-        <v>43201</v>
+        <v>45546</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -2020,10 +2020,10 @@
         <v>74</v>
       </c>
       <c r="B6" s="4">
-        <v>43112</v>
+        <v>45468</v>
       </c>
       <c r="C6" s="4">
-        <v>43143</v>
+        <v>45470</v>
       </c>
     </row>
   </sheetData>
@@ -2099,7 +2099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A737D97F-C3F3-4EBB-935E-89B1E56B6C13}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -2371,10 +2371,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63ECF564-DD6A-47B3-9FA7-B9A0B7520F7A}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2402,10 +2402,10 @@
         <v>53</v>
       </c>
       <c r="B2" s="4">
-        <v>43162</v>
+        <v>45466</v>
       </c>
       <c r="C2" s="4">
-        <v>43193</v>
+        <v>45471</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -2413,10 +2413,10 @@
         <v>55</v>
       </c>
       <c r="B3" s="4">
-        <v>43198</v>
+        <v>45573</v>
       </c>
       <c r="C3" s="4">
-        <v>43228</v>
+        <v>45575</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2424,10 +2424,10 @@
         <v>54</v>
       </c>
       <c r="B4" s="4">
-        <v>43109</v>
+        <v>45631</v>
       </c>
       <c r="C4" s="4">
-        <v>43140</v>
+        <v>45639</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2435,10 +2435,10 @@
         <v>53</v>
       </c>
       <c r="B5" s="4">
-        <v>43170</v>
+        <v>45605</v>
       </c>
       <c r="C5" s="4">
-        <v>43201</v>
+        <v>45606</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -2446,11 +2446,14 @@
         <v>54</v>
       </c>
       <c r="B6" s="4">
-        <v>43112</v>
+        <v>45503</v>
       </c>
       <c r="C6" s="4">
-        <v>43143</v>
-      </c>
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2462,7 +2465,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C10" sqref="C6:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2514,7 +2517,7 @@
         <v>33</v>
       </c>
       <c r="C4" s="4">
-        <v>45578</v>
+        <v>45639</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2580,7 +2583,7 @@
         <v>28</v>
       </c>
       <c r="C10" s="4">
-        <v>45443</v>
+        <v>45470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>